<commit_message>
Major project status updated...
</commit_message>
<xml_diff>
--- a/Documents/Daily Status.xlsx
+++ b/Documents/Daily Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="815" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="815" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="475">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -392,9 +392,6 @@
     <t>Shankar Kumar</t>
   </si>
   <si>
-    <t>No Status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Damping control </t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t>Sushil Kumar</t>
   </si>
   <si>
-    <t>In Progress : setup for base</t>
-  </si>
-  <si>
     <t xml:space="preserve">Robotics Kits </t>
   </si>
   <si>
@@ -453,9 +447,6 @@
   </si>
   <si>
     <t>Sohan</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t xml:space="preserve">Wireless mobile charger </t>
@@ -501,15 +492,6 @@
     <t>Galgotia</t>
   </si>
   <si>
-    <t>Mobile bug and mobile jammer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shyam dixit </t>
-  </si>
-  <si>
-    <t>G.L.Bajaj</t>
-  </si>
-  <si>
     <t xml:space="preserve">MOBILE DETECTOR WITH JAMMER </t>
   </si>
   <si>
@@ -519,13 +501,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Project Report given</t>
-  </si>
-  <si>
     <t>3 students from south</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Progress </t>
   </si>
   <si>
     <t xml:space="preserve">Xbee Protocol Based Project </t>
@@ -3852,6 +3828,24 @@
       </rPr>
       <t>AT89S52 based IC Tester with Visual Basic  (1200/-)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">They had gone their home town they will come in feb  </t>
+  </si>
+  <si>
+    <t>They will come in feb</t>
+  </si>
+  <si>
+    <t>Course has been completed</t>
+  </si>
+  <si>
+    <t>They will come day afetr tomorrow.</t>
+  </si>
+  <si>
+    <t>PCB Design has been completed on Eagle win .</t>
+  </si>
+  <si>
+    <t>Project has been successfully delivered to the client.</t>
   </si>
 </sst>
 </file>
@@ -3923,7 +3917,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3963,6 +3957,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4056,7 +4056,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4153,9 +4153,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4167,9 +4164,6 @@
     </xf>
     <xf numFmtId="15" fontId="2" fillId="7" borderId="5" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
@@ -4207,6 +4201,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4563,36 +4577,36 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="63" customFormat="1">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:11" s="61" customFormat="1">
+      <c r="A2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="61">
         <v>9540890120</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="64">
+      <c r="H2" s="62">
         <v>42016</v>
       </c>
-      <c r="J2" s="63" t="s">
-        <v>181</v>
-      </c>
-      <c r="K2" s="63" t="s">
-        <v>458</v>
+      <c r="J2" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="61" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4624,7 +4638,7 @@
         <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4640,7 +4654,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4880,22 +4894,22 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B10">
         <v>8800934802</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="D10" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="E10" t="s">
         <v>109</v>
       </c>
       <c r="F10" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="G10" t="s">
         <v>41</v>
@@ -4906,25 +4920,25 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B11">
         <v>9971564923</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="D11" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="E11" t="s">
         <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="G11" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="H11" t="s">
         <v>44</v>
@@ -4932,39 +4946,39 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B12">
         <v>9871310918</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D12" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="E12" t="s">
         <v>109</v>
       </c>
       <c r="F12" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B13">
         <v>9582449984</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
@@ -5178,7 +5192,7 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5211,7 +5225,7 @@
         <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5260,49 +5274,49 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B6" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B7" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="C7" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B8" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="63" customFormat="1">
-      <c r="A9" s="63" t="s">
-        <v>450</v>
-      </c>
-      <c r="B9" s="63" t="s">
-        <v>456</v>
-      </c>
-      <c r="C9" s="63" t="s">
+    <row r="9" spans="1:4" s="61" customFormat="1">
+      <c r="A9" s="61" t="s">
+        <v>442</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="63" t="s">
-        <v>467</v>
+      <c r="D9" s="61" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -5424,15 +5438,15 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B14" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -5442,11 +5456,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6164,7 +6178,7 @@
         <v>112</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>113</v>
@@ -6196,7 +6210,7 @@
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:12" s="22" customFormat="1" ht="13.5" thickBot="1">
+    <row r="3" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -6222,58 +6236,58 @@
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="L3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" s="71" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A4" s="64">
+        <v>2</v>
+      </c>
+      <c r="B4" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="L3" s="21"/>
-    </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A4" s="23">
-        <v>2</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="66">
+        <v>41924</v>
+      </c>
+      <c r="D4" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="25">
-        <v>41924</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="E4" s="68"/>
+      <c r="F4" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="28">
+      <c r="G4" s="69">
         <v>9999405538</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="64">
         <v>7000</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="64">
         <v>500</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="L4" s="29"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="68" t="s">
+        <v>469</v>
+      </c>
+      <c r="L4" s="70"/>
     </row>
     <row r="5" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1">
       <c r="A5" s="31">
         <v>3</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="33">
         <v>41947</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="35"/>
       <c r="F5" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G5" s="36">
         <v>9650182218</v>
@@ -6286,7 +6300,7 @@
       </c>
       <c r="J5" s="31"/>
       <c r="K5" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L5" s="38"/>
     </row>
@@ -6295,13 +6309,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="25">
         <v>41947</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="28" t="s">
@@ -6318,7 +6332,7 @@
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="27" t="s">
-        <v>133</v>
+        <v>470</v>
       </c>
       <c r="L6" s="29"/>
     </row>
@@ -6327,17 +6341,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C7" s="33">
         <v>41907</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G7" s="36">
         <v>9891085793</v>
@@ -6350,7 +6364,7 @@
       </c>
       <c r="J7" s="31"/>
       <c r="K7" s="35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L7" s="38"/>
     </row>
@@ -6359,17 +6373,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8" s="33">
         <v>41947</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G8" s="36">
         <v>9350215064</v>
@@ -6382,7 +6396,7 @@
       </c>
       <c r="J8" s="31"/>
       <c r="K8" s="35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L8" s="38"/>
     </row>
@@ -6391,13 +6405,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="33">
         <v>41952</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="36"/>
@@ -6412,7 +6426,7 @@
       </c>
       <c r="J9" s="31"/>
       <c r="K9" s="35" t="s">
-        <v>144</v>
+        <v>471</v>
       </c>
       <c r="L9" s="38"/>
     </row>
@@ -6421,13 +6435,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C10" s="33">
         <v>41964</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="36"/>
@@ -6442,7 +6456,7 @@
       </c>
       <c r="J10" s="31"/>
       <c r="K10" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L10" s="38"/>
     </row>
@@ -6451,17 +6465,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C11" s="33">
         <v>41964</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G11" s="36">
         <v>9958911395</v>
@@ -6476,7 +6490,7 @@
         <v>41971</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L11" s="38"/>
     </row>
@@ -6485,17 +6499,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" s="25">
         <v>41964</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G12" s="28">
         <v>8527336673</v>
@@ -6508,22 +6522,22 @@
       </c>
       <c r="J12" s="23"/>
       <c r="K12" s="41" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="1:12" s="22" customFormat="1" ht="13.5" thickBot="1">
+    <row r="13" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
       <c r="A13" s="16">
         <v>11</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C13" s="18">
         <v>41947</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="17" t="s">
@@ -6540,26 +6554,26 @@
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="20" t="s">
-        <v>123</v>
+        <v>469</v>
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" s="22" customFormat="1" ht="13.5" thickBot="1">
+    <row r="14" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
       <c r="A14" s="16">
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" s="18">
         <v>41947</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G14" s="17">
         <v>7042060502</v>
@@ -6572,231 +6586,199 @@
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="20" t="s">
-        <v>123</v>
+        <v>472</v>
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" s="22" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A15" s="16">
-        <v>13</v>
-      </c>
-      <c r="B15" s="42" t="s">
+    <row r="15" spans="1:12" s="30" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A15" s="23">
+        <v>14</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="25">
+        <v>41983</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28">
+        <v>8287414627</v>
+      </c>
+      <c r="H15" s="23">
+        <v>4000</v>
+      </c>
+      <c r="I15" s="23">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="68" t="s">
+        <v>469</v>
+      </c>
+      <c r="L15" s="29"/>
+    </row>
+    <row r="16" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A16" s="31">
+        <v>15</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="33">
+        <v>41980</v>
+      </c>
+      <c r="D16" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="18">
-        <v>41977</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="G15" s="17">
-        <v>9458855376</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-      <c r="I15" s="16">
-        <v>0</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="L15" s="21"/>
-    </row>
-    <row r="16" spans="1:12" s="30" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A16" s="23">
-        <v>14</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="25">
-        <v>41983</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28">
-        <v>8287414627</v>
-      </c>
-      <c r="H16" s="23">
-        <v>4000</v>
-      </c>
-      <c r="I16" s="23">
-        <v>1000</v>
-      </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="L16" s="29"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="31">
+        <v>4500</v>
+      </c>
+      <c r="I16" s="31">
+        <v>1500</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="37" t="s">
+        <v>473</v>
+      </c>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A17" s="31">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="C17" s="33">
-        <v>41980</v>
+        <v>41985</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
+        <v>161</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="36" t="s">
+        <v>163</v>
+      </c>
       <c r="H17" s="31">
-        <v>4500</v>
+        <v>5800</v>
       </c>
       <c r="I17" s="31">
-        <v>1500</v>
+        <v>5800</v>
       </c>
       <c r="J17" s="31"/>
       <c r="K17" s="37" t="s">
+        <v>474</v>
+      </c>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="1:12" s="47" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A18" s="43">
+        <v>17</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="45">
+        <v>41987</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="L17" s="38"/>
-    </row>
-    <row r="18" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A18" s="31">
-        <v>16</v>
-      </c>
-      <c r="B18" s="36" t="s">
+      <c r="H18" s="43">
+        <v>4000</v>
+      </c>
+      <c r="I18" s="43">
+        <v>4000</v>
+      </c>
+      <c r="J18" s="43"/>
+      <c r="K18" s="37" t="s">
+        <v>474</v>
+      </c>
+      <c r="L18" s="46"/>
+    </row>
+    <row r="19" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
+      <c r="A19" s="31">
+        <v>19</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="33">
-        <v>41985</v>
-      </c>
-      <c r="D18" s="36" t="s">
+      <c r="C19" s="33">
+        <v>42020</v>
+      </c>
+      <c r="D19" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E19" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="36" t="s">
+      <c r="F19" s="36"/>
+      <c r="G19" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="H18" s="31">
-        <v>5800</v>
-      </c>
-      <c r="I18" s="31">
-        <v>5800</v>
-      </c>
-      <c r="J18" s="31"/>
-      <c r="K18" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="L18" s="38"/>
-    </row>
-    <row r="19" spans="1:12" s="49" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A19" s="44">
-        <v>17</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="46">
-        <v>41987</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H19" s="44">
-        <v>4000</v>
-      </c>
-      <c r="I19" s="44">
-        <v>4000</v>
-      </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="L19" s="48"/>
-    </row>
-    <row r="20" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A20" s="31">
-        <v>19</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="33">
-        <v>42020</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="E20" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="H20" s="31">
+      <c r="H19" s="31">
         <v>3000</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I19" s="31">
         <v>3000</v>
       </c>
-      <c r="J20" s="31"/>
-      <c r="K20" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="1:12" s="54" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="53"/>
-    </row>
-    <row r="22" spans="1:12" s="54" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="53"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="L19" s="38"/>
+    </row>
+    <row r="20" spans="1:12" s="52" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12" s="52" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="51"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E19" r:id="rId1"/>
+    <hyperlink ref="E18" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6807,1390 +6789,1390 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="84.85546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.85546875" style="59" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="15" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="54"/>
+      <c r="D2" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5">
+      <c r="A3" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="15" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="54" t="s">
         <v>186</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="56"/>
-      <c r="D2" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5">
-      <c r="A3" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" s="56" t="s">
-        <v>194</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" s="54" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6" s="56" t="s">
+      <c r="D8" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="15" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="A7" s="56" t="s">
+      <c r="D9" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="15" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="56" t="s">
         <v>200</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8" s="56" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="56" t="s">
-        <v>205</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="58" t="s">
-        <v>208</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>94</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15">
-      <c r="A11" s="56" t="s">
-        <v>210</v>
+      <c r="A11" s="54" t="s">
+        <v>202</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15">
-      <c r="A12" s="56" t="s">
-        <v>212</v>
+      <c r="A12" s="54" t="s">
+        <v>204</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>94</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" s="57" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15">
+      <c r="A15" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="54" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="A13" s="59" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="A14" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="A15" s="56" t="s">
-        <v>216</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15">
-      <c r="A16" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
-      <c r="A17" s="59" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15">
-      <c r="A19" s="56" t="s">
-        <v>221</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="56" t="s">
-        <v>222</v>
+      <c r="A20" s="54" t="s">
+        <v>214</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
-      <c r="A21" s="56" t="s">
-        <v>223</v>
+      <c r="A21" s="54" t="s">
+        <v>215</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15">
-      <c r="A22" s="56" t="s">
-        <v>225</v>
+      <c r="A22" s="54" t="s">
+        <v>217</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15">
-      <c r="A23" s="56" t="s">
-        <v>227</v>
+      <c r="A23" s="54" t="s">
+        <v>219</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15">
-      <c r="A24" s="56" t="s">
-        <v>229</v>
+      <c r="A24" s="54" t="s">
+        <v>221</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15">
-      <c r="A25" s="56" t="s">
-        <v>460</v>
+      <c r="A25" s="54" t="s">
+        <v>452</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="54" t="s">
+        <v>454</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
-      <c r="A27" s="56" t="s">
-        <v>471</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>470</v>
-      </c>
     </row>
     <row r="28" spans="1:3" ht="15">
-      <c r="A28" s="56" t="s">
-        <v>473</v>
+      <c r="A28" s="54" t="s">
+        <v>465</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15">
-      <c r="A29" s="56" t="s">
-        <v>474</v>
+      <c r="A29" s="54" t="s">
+        <v>466</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
-      <c r="A30" s="56" t="s">
-        <v>475</v>
+      <c r="A30" s="54" t="s">
+        <v>467</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="65" customFormat="1" ht="15">
-      <c r="A31" s="59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="63" customFormat="1" ht="15">
+      <c r="A31" s="57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15">
+      <c r="A33" s="54" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15">
+      <c r="A34" s="54" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15">
+      <c r="A35" s="54" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15">
+      <c r="A36" s="54" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15">
+      <c r="A37" s="54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15">
+      <c r="A38" s="54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15">
+      <c r="A39" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15">
+      <c r="A40" s="54" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="56" t="s">
-        <v>476</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15">
-      <c r="A33" s="56" t="s">
+    <row r="41" spans="1:1" ht="15">
+      <c r="A41" s="54" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15">
-      <c r="A34" s="56" t="s">
+    <row r="42" spans="1:1" ht="15">
+      <c r="A42" s="54" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15">
-      <c r="A35" s="56" t="s">
+    <row r="43" spans="1:1" ht="15">
+      <c r="A43" s="54" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15">
-      <c r="A36" s="56" t="s">
+    <row r="44" spans="1:1" ht="15">
+      <c r="A44" s="54" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15">
-      <c r="A37" s="56" t="s">
+    <row r="45" spans="1:1" ht="15">
+      <c r="A45" s="54" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15">
-      <c r="A38" s="56" t="s">
+    <row r="46" spans="1:1" ht="15">
+      <c r="A46" s="54" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15">
-      <c r="A39" s="56" t="s">
+    <row r="47" spans="1:1" ht="15">
+      <c r="A47" s="54" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15">
-      <c r="A40" s="56" t="s">
+    <row r="48" spans="1:1" ht="15">
+      <c r="A48" s="54" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15">
-      <c r="A41" s="56" t="s">
+    <row r="49" spans="1:1" ht="15">
+      <c r="A49" s="54" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15">
-      <c r="A42" s="56" t="s">
+    <row r="50" spans="1:1" ht="15">
+      <c r="A50" s="54" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15">
-      <c r="A43" s="56" t="s">
+    <row r="51" spans="1:1" ht="15">
+      <c r="A51" s="58"/>
+    </row>
+    <row r="52" spans="1:1" ht="15">
+      <c r="A52" s="54"/>
+    </row>
+    <row r="53" spans="1:1" ht="16.5">
+      <c r="A53" s="55" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15">
-      <c r="A44" s="56" t="s">
+    <row r="54" spans="1:1" ht="15">
+      <c r="A54" s="54" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15">
-      <c r="A45" s="56" t="s">
+    <row r="55" spans="1:1" ht="15">
+      <c r="A55" s="54" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15">
-      <c r="A46" s="56" t="s">
+    <row r="56" spans="1:1" ht="15">
+      <c r="A56" s="54" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15">
-      <c r="A47" s="56" t="s">
+    <row r="57" spans="1:1" ht="15">
+      <c r="A57" s="54" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15">
-      <c r="A48" s="56" t="s">
+    <row r="58" spans="1:1" ht="15">
+      <c r="A58" s="54" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15">
-      <c r="A49" s="56" t="s">
+    <row r="59" spans="1:1" ht="15">
+      <c r="A59" s="54" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15">
-      <c r="A50" s="56" t="s">
+    <row r="60" spans="1:1" ht="15">
+      <c r="A60" s="54" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15">
-      <c r="A51" s="60"/>
-    </row>
-    <row r="52" spans="1:1" ht="15">
-      <c r="A52" s="56"/>
-    </row>
-    <row r="53" spans="1:1" ht="16.5">
-      <c r="A53" s="57" t="s">
+    <row r="61" spans="1:1" ht="15">
+      <c r="A61" s="54" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15">
-      <c r="A54" s="56" t="s">
+    <row r="62" spans="1:1" ht="15">
+      <c r="A62" s="54" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15">
-      <c r="A55" s="56" t="s">
+    <row r="63" spans="1:1" ht="15">
+      <c r="A63" s="54" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15">
-      <c r="A56" s="56" t="s">
+    <row r="64" spans="1:1" ht="15">
+      <c r="A64" s="54" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15">
-      <c r="A57" s="56" t="s">
+    <row r="65" spans="1:1" ht="15">
+      <c r="A65" s="54" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15">
-      <c r="A58" s="56" t="s">
+    <row r="66" spans="1:1" ht="15">
+      <c r="A66" s="54" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15">
-      <c r="A59" s="56" t="s">
+    <row r="67" spans="1:1" ht="15">
+      <c r="A67" s="54" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15">
-      <c r="A60" s="56" t="s">
+    <row r="68" spans="1:1" ht="15">
+      <c r="A68" s="54" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15">
-      <c r="A61" s="56" t="s">
+    <row r="69" spans="1:1" ht="15">
+      <c r="A69" s="54" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15">
-      <c r="A62" s="56" t="s">
+    <row r="70" spans="1:1" ht="15">
+      <c r="A70" s="54" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15">
-      <c r="A63" s="56" t="s">
+    <row r="71" spans="1:1" ht="15">
+      <c r="A71" s="54" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15">
-      <c r="A64" s="56" t="s">
+    <row r="72" spans="1:1" ht="15">
+      <c r="A72" s="54" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15">
-      <c r="A65" s="56" t="s">
+    <row r="73" spans="1:1" ht="15">
+      <c r="A73" s="54" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15">
-      <c r="A66" s="56" t="s">
+    <row r="74" spans="1:1" ht="15">
+      <c r="A74" s="54" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15">
-      <c r="A67" s="56" t="s">
+    <row r="75" spans="1:1" ht="15">
+      <c r="A75" s="54" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15">
-      <c r="A68" s="56" t="s">
+    <row r="76" spans="1:1" ht="15">
+      <c r="A76" s="54" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="15">
-      <c r="A69" s="56" t="s">
+    <row r="77" spans="1:1" ht="15">
+      <c r="A77" s="54"/>
+    </row>
+    <row r="78" spans="1:1" ht="16.5">
+      <c r="A78" s="55" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="15">
-      <c r="A70" s="56" t="s">
+    <row r="79" spans="1:1" ht="15">
+      <c r="A79" s="54" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="15">
-      <c r="A71" s="56" t="s">
+    <row r="80" spans="1:1" ht="15">
+      <c r="A80" s="54" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="15">
-      <c r="A72" s="56" t="s">
+    <row r="81" spans="1:1" ht="15">
+      <c r="A81" s="54" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="15">
-      <c r="A73" s="56" t="s">
+    <row r="82" spans="1:1" ht="15">
+      <c r="A82" s="54" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="15">
-      <c r="A74" s="56" t="s">
+    <row r="83" spans="1:1" ht="15">
+      <c r="A83" s="54" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="15">
-      <c r="A75" s="56" t="s">
+    <row r="84" spans="1:1" ht="15">
+      <c r="A84" s="54" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15">
-      <c r="A76" s="56" t="s">
+    <row r="85" spans="1:1" ht="15">
+      <c r="A85" s="54" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="15">
-      <c r="A77" s="56"/>
-    </row>
-    <row r="78" spans="1:1" ht="16.5">
-      <c r="A78" s="57" t="s">
+    <row r="86" spans="1:1" ht="15">
+      <c r="A86" s="54" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="15">
-      <c r="A79" s="56" t="s">
+    <row r="87" spans="1:1" ht="15">
+      <c r="A87" s="54" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="15">
-      <c r="A80" s="56" t="s">
+    <row r="88" spans="1:1" ht="15">
+      <c r="A88" s="54" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15">
-      <c r="A81" s="56" t="s">
+    <row r="89" spans="1:1" ht="15">
+      <c r="A89" s="54" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15">
-      <c r="A82" s="56" t="s">
+    <row r="90" spans="1:1" ht="15">
+      <c r="A90" s="54" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15">
-      <c r="A83" s="56" t="s">
+    <row r="91" spans="1:1" ht="15">
+      <c r="A91" s="54" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15">
-      <c r="A84" s="56" t="s">
+    <row r="92" spans="1:1" ht="15">
+      <c r="A92" s="54" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15">
-      <c r="A85" s="56" t="s">
+    <row r="93" spans="1:1" ht="15">
+      <c r="A93" s="54" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15">
-      <c r="A86" s="56" t="s">
+    <row r="94" spans="1:1" ht="15">
+      <c r="A94" s="54" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15">
-      <c r="A87" s="56" t="s">
+    <row r="95" spans="1:1" ht="15">
+      <c r="A95" s="54" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15">
-      <c r="A88" s="56" t="s">
+    <row r="96" spans="1:1" ht="15">
+      <c r="A96" s="54" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15">
-      <c r="A89" s="56" t="s">
+    <row r="97" spans="1:1" ht="15">
+      <c r="A97" s="54" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15">
-      <c r="A90" s="56" t="s">
+    <row r="98" spans="1:1" ht="15">
+      <c r="A98" s="54" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15">
-      <c r="A91" s="56" t="s">
+    <row r="99" spans="1:1" ht="15">
+      <c r="A99" s="54" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15">
-      <c r="A92" s="56" t="s">
+    <row r="100" spans="1:1" ht="15">
+      <c r="A100" s="54" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15">
-      <c r="A93" s="56" t="s">
+    <row r="101" spans="1:1" ht="15">
+      <c r="A101" s="54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15">
-      <c r="A94" s="56" t="s">
+    <row r="102" spans="1:1" ht="15">
+      <c r="A102" s="54" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15">
-      <c r="A95" s="56" t="s">
+    <row r="103" spans="1:1" ht="15">
+      <c r="A103" s="54" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15">
-      <c r="A96" s="56" t="s">
+    <row r="104" spans="1:1" ht="15">
+      <c r="A104" s="54" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="15">
-      <c r="A97" s="56" t="s">
+    <row r="105" spans="1:1" ht="15">
+      <c r="A105" s="54" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="15">
-      <c r="A98" s="56" t="s">
+    <row r="106" spans="1:1" ht="15">
+      <c r="A106" s="54" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="15">
+      <c r="A107" s="54"/>
+    </row>
+    <row r="108" spans="1:1" ht="16.5">
+      <c r="A108" s="55" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="15">
-      <c r="A99" s="56" t="s">
+    <row r="109" spans="1:1" ht="15">
+      <c r="A109" s="54" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="15">
-      <c r="A100" s="56" t="s">
+    <row r="110" spans="1:1" ht="15">
+      <c r="A110" s="54" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="15">
-      <c r="A101" s="56" t="s">
+    <row r="111" spans="1:1" ht="15">
+      <c r="A111" s="54" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="15">
-      <c r="A102" s="56" t="s">
+    <row r="112" spans="1:1" ht="15">
+      <c r="A112" s="54" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="15">
-      <c r="A103" s="56" t="s">
+    <row r="113" spans="1:1" ht="15">
+      <c r="A113" s="54" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="15">
-      <c r="A104" s="56" t="s">
+    <row r="114" spans="1:1" ht="15">
+      <c r="A114" s="54" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="15">
-      <c r="A105" s="56" t="s">
+    <row r="115" spans="1:1" ht="15">
+      <c r="A115" s="54" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="15">
-      <c r="A106" s="56" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" ht="15">
-      <c r="A107" s="56"/>
-    </row>
-    <row r="108" spans="1:1" ht="16.5">
-      <c r="A108" s="57" t="s">
+    <row r="116" spans="1:1" ht="15">
+      <c r="A116" s="54" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="15">
-      <c r="A109" s="56" t="s">
+    <row r="117" spans="1:1" ht="15">
+      <c r="A117" s="54" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="15">
-      <c r="A110" s="56" t="s">
+    <row r="118" spans="1:1" ht="15">
+      <c r="A118" s="54" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="15">
-      <c r="A111" s="56" t="s">
+    <row r="119" spans="1:1" ht="15">
+      <c r="A119" s="54" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="15">
-      <c r="A112" s="56" t="s">
+    <row r="120" spans="1:1" ht="15">
+      <c r="A120" s="54" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="15">
-      <c r="A113" s="56" t="s">
+    <row r="121" spans="1:1" ht="15">
+      <c r="A121" s="54" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="15">
-      <c r="A114" s="56" t="s">
+    <row r="122" spans="1:1" ht="15">
+      <c r="A122" s="54" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="15">
+      <c r="A123" s="54"/>
+    </row>
+    <row r="124" spans="1:1" ht="16.5">
+      <c r="A124" s="55" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="15">
-      <c r="A115" s="56" t="s">
+    <row r="125" spans="1:1" ht="15">
+      <c r="A125" s="54" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="15">
-      <c r="A116" s="56" t="s">
+    <row r="126" spans="1:1" ht="15">
+      <c r="A126" s="54" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="15">
-      <c r="A117" s="56" t="s">
+    <row r="127" spans="1:1" ht="15">
+      <c r="A127" s="54" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="15">
-      <c r="A118" s="56" t="s">
+    <row r="128" spans="1:1" ht="15">
+      <c r="A128" s="54" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="15">
-      <c r="A119" s="56" t="s">
+    <row r="129" spans="1:1" ht="15">
+      <c r="A129" s="54" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="15">
-      <c r="A120" s="56" t="s">
+    <row r="130" spans="1:1" ht="15">
+      <c r="A130" s="54" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="15">
-      <c r="A121" s="56" t="s">
+    <row r="131" spans="1:1" ht="15">
+      <c r="A131" s="54" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="15">
-      <c r="A122" s="56" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" ht="15">
-      <c r="A123" s="56"/>
-    </row>
-    <row r="124" spans="1:1" ht="16.5">
-      <c r="A124" s="57" t="s">
+    <row r="132" spans="1:1" ht="15">
+      <c r="A132" s="54" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="15">
-      <c r="A125" s="56" t="s">
+    <row r="133" spans="1:1" ht="15">
+      <c r="A133" s="54" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="15">
-      <c r="A126" s="56" t="s">
+    <row r="134" spans="1:1" ht="15">
+      <c r="A134" s="54" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="15">
-      <c r="A127" s="56" t="s">
+    <row r="135" spans="1:1" ht="15">
+      <c r="A135" s="54" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="15">
-      <c r="A128" s="56" t="s">
+    <row r="136" spans="1:1" ht="15">
+      <c r="A136" s="54" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="15">
-      <c r="A129" s="56" t="s">
+    <row r="137" spans="1:1" ht="15">
+      <c r="A137" s="54" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="15">
-      <c r="A130" s="56" t="s">
+    <row r="138" spans="1:1" ht="15">
+      <c r="A138" s="54" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="15">
-      <c r="A131" s="56" t="s">
+    <row r="139" spans="1:1" ht="15">
+      <c r="A139" s="54" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="15">
-      <c r="A132" s="56" t="s">
+    <row r="140" spans="1:1" ht="15">
+      <c r="A140" s="54" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="15">
-      <c r="A133" s="56" t="s">
+    <row r="141" spans="1:1" ht="15">
+      <c r="A141" s="54" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="15">
-      <c r="A134" s="56" t="s">
+    <row r="142" spans="1:1" ht="15">
+      <c r="A142" s="54" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="15">
-      <c r="A135" s="56" t="s">
+    <row r="143" spans="1:1" ht="15">
+      <c r="A143" s="54" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="15">
-      <c r="A136" s="56" t="s">
+    <row r="144" spans="1:1" ht="15">
+      <c r="A144" s="54" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="15">
-      <c r="A137" s="56" t="s">
+    <row r="145" spans="1:1" ht="15">
+      <c r="A145" s="54" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="15">
-      <c r="A138" s="56" t="s">
+    <row r="146" spans="1:1" ht="15">
+      <c r="A146" s="54" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="15">
-      <c r="A139" s="56" t="s">
+    <row r="147" spans="1:1" ht="15">
+      <c r="A147" s="54" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="15">
-      <c r="A140" s="56" t="s">
+    <row r="148" spans="1:1" ht="15">
+      <c r="A148" s="54" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="15">
-      <c r="A141" s="56" t="s">
+    <row r="149" spans="1:1" ht="15">
+      <c r="A149" s="54" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="15">
-      <c r="A142" s="56" t="s">
+    <row r="150" spans="1:1" ht="15">
+      <c r="A150" s="54" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="15">
-      <c r="A143" s="56" t="s">
+    <row r="151" spans="1:1" ht="15">
+      <c r="A151" s="54" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="15">
-      <c r="A144" s="56" t="s">
+    <row r="152" spans="1:1" ht="15">
+      <c r="A152" s="54" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="15">
-      <c r="A145" s="56" t="s">
+    <row r="153" spans="1:1" ht="15">
+      <c r="A153" s="54" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="15">
-      <c r="A146" s="56" t="s">
+    <row r="154" spans="1:1" ht="15">
+      <c r="A154" s="54" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="15">
-      <c r="A147" s="56" t="s">
+    <row r="155" spans="1:1" ht="15">
+      <c r="A155" s="54"/>
+    </row>
+    <row r="156" spans="1:1" ht="16.5">
+      <c r="A156" s="55" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="15">
-      <c r="A148" s="56" t="s">
+    <row r="157" spans="1:1" ht="15">
+      <c r="A157" s="54" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="15">
-      <c r="A149" s="56" t="s">
+    <row r="158" spans="1:1" ht="15">
+      <c r="A158" s="54" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="15">
-      <c r="A150" s="56" t="s">
+    <row r="159" spans="1:1" ht="15">
+      <c r="A159" s="54" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="15">
-      <c r="A151" s="56" t="s">
+    <row r="160" spans="1:1" ht="15">
+      <c r="A160" s="54" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="15">
-      <c r="A152" s="56" t="s">
+    <row r="161" spans="1:1" ht="15">
+      <c r="A161" s="54" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="15">
-      <c r="A153" s="56" t="s">
+    <row r="162" spans="1:1" ht="15">
+      <c r="A162" s="54" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="15">
-      <c r="A154" s="56" t="s">
+    <row r="163" spans="1:1" ht="15">
+      <c r="A163" s="54" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="16.5">
+      <c r="A164" s="55" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="15">
-      <c r="A155" s="56"/>
-    </row>
-    <row r="156" spans="1:1" ht="16.5">
-      <c r="A156" s="57" t="s">
+    <row r="165" spans="1:1" ht="15">
+      <c r="A165" s="54" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="15">
-      <c r="A157" s="56" t="s">
+    <row r="166" spans="1:1" ht="15">
+      <c r="A166" s="54" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="15">
-      <c r="A158" s="56" t="s">
+    <row r="167" spans="1:1" ht="15">
+      <c r="A167" s="54" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="15">
-      <c r="A159" s="56" t="s">
+    <row r="168" spans="1:1" ht="15">
+      <c r="A168" s="54" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="15">
-      <c r="A160" s="56" t="s">
+    <row r="169" spans="1:1" ht="15">
+      <c r="A169" s="54" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="15">
-      <c r="A161" s="56" t="s">
+    <row r="170" spans="1:1" ht="15">
+      <c r="A170" s="54" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="15">
-      <c r="A162" s="56" t="s">
+    <row r="171" spans="1:1" ht="15">
+      <c r="A171" s="54" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="15">
-      <c r="A163" s="56" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" ht="16.5">
-      <c r="A164" s="57" t="s">
+    <row r="172" spans="1:1" ht="15">
+      <c r="A172" s="54" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="15">
-      <c r="A165" s="56" t="s">
+    <row r="173" spans="1:1" ht="15">
+      <c r="A173" s="54" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="15">
-      <c r="A166" s="56" t="s">
+    <row r="174" spans="1:1" ht="15">
+      <c r="A174" s="54" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="15">
-      <c r="A167" s="56" t="s">
+    <row r="175" spans="1:1" ht="15">
+      <c r="A175" s="54" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="15">
-      <c r="A168" s="56" t="s">
+    <row r="176" spans="1:1" ht="15">
+      <c r="A176" s="54" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="15">
-      <c r="A169" s="56" t="s">
+    <row r="177" spans="1:1" ht="15">
+      <c r="A177" s="54" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="15">
-      <c r="A170" s="56" t="s">
+    <row r="178" spans="1:1" ht="15">
+      <c r="A178" s="54" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="15">
-      <c r="A171" s="56" t="s">
+    <row r="179" spans="1:1" ht="15">
+      <c r="A179" s="54" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="15">
-      <c r="A172" s="56" t="s">
+    <row r="180" spans="1:1" ht="15">
+      <c r="A180" s="54" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="15">
-      <c r="A173" s="56" t="s">
+    <row r="181" spans="1:1" ht="15">
+      <c r="A181" s="54" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="15">
-      <c r="A174" s="56" t="s">
+    <row r="182" spans="1:1" ht="15">
+      <c r="A182" s="54" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="15">
-      <c r="A175" s="56" t="s">
+    <row r="183" spans="1:1" ht="15">
+      <c r="A183" s="54" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="15">
-      <c r="A176" s="56" t="s">
+    <row r="184" spans="1:1" ht="15">
+      <c r="A184" s="54" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="15">
-      <c r="A177" s="56" t="s">
+    <row r="185" spans="1:1" ht="15">
+      <c r="A185" s="54" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="15">
-      <c r="A178" s="56" t="s">
+    <row r="186" spans="1:1" ht="15">
+      <c r="A186" s="54" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="15">
-      <c r="A179" s="56" t="s">
+    <row r="187" spans="1:1" ht="15">
+      <c r="A187" s="54" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="15">
-      <c r="A180" s="56" t="s">
+    <row r="188" spans="1:1" ht="15">
+      <c r="A188" s="54" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="15">
-      <c r="A181" s="56" t="s">
+    <row r="189" spans="1:1" ht="15">
+      <c r="A189" s="54" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="15">
-      <c r="A182" s="56" t="s">
+    <row r="190" spans="1:1" ht="15">
+      <c r="A190" s="54" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="15">
-      <c r="A183" s="56" t="s">
+    <row r="191" spans="1:1" ht="15">
+      <c r="A191" s="54" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="15">
-      <c r="A184" s="56" t="s">
+    <row r="192" spans="1:1" ht="15">
+      <c r="A192" s="54" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="15">
-      <c r="A185" s="56" t="s">
+    <row r="193" spans="1:1" ht="15">
+      <c r="A193" s="54" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="15">
-      <c r="A186" s="56" t="s">
+    <row r="194" spans="1:1" ht="15">
+      <c r="A194" s="54" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="15">
-      <c r="A187" s="56" t="s">
+    <row r="195" spans="1:1" ht="15">
+      <c r="A195" s="54" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="15">
-      <c r="A188" s="56" t="s">
+    <row r="196" spans="1:1" ht="15">
+      <c r="A196" s="54" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="15">
-      <c r="A189" s="56" t="s">
+    <row r="197" spans="1:1" ht="15">
+      <c r="A197" s="54" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="15">
-      <c r="A190" s="56" t="s">
+    <row r="198" spans="1:1" ht="15">
+      <c r="A198" s="54" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="15">
-      <c r="A191" s="56" t="s">
+    <row r="199" spans="1:1" ht="15">
+      <c r="A199" s="54"/>
+    </row>
+    <row r="200" spans="1:1" ht="16.5">
+      <c r="A200" s="55" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="15">
-      <c r="A192" s="56" t="s">
+    <row r="201" spans="1:1" ht="15">
+      <c r="A201" s="54" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="15">
-      <c r="A193" s="56" t="s">
+    <row r="202" spans="1:1" ht="15">
+      <c r="A202" s="54" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="15">
-      <c r="A194" s="56" t="s">
+    <row r="203" spans="1:1" ht="15">
+      <c r="A203" s="54" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="15">
-      <c r="A195" s="56" t="s">
+    <row r="204" spans="1:1" ht="15">
+      <c r="A204" s="54" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="15">
-      <c r="A196" s="56" t="s">
+    <row r="205" spans="1:1" ht="15">
+      <c r="A205" s="54" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="15">
-      <c r="A197" s="56" t="s">
+    <row r="206" spans="1:1" ht="15">
+      <c r="A206" s="54" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="15">
-      <c r="A198" s="56" t="s">
+    <row r="207" spans="1:1" ht="15">
+      <c r="A207" s="54" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="15">
-      <c r="A199" s="56"/>
-    </row>
-    <row r="200" spans="1:1" ht="16.5">
-      <c r="A200" s="57" t="s">
+    <row r="208" spans="1:1" ht="15">
+      <c r="A208" s="54" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="15">
-      <c r="A201" s="56" t="s">
+    <row r="209" spans="1:1" ht="15">
+      <c r="A209" s="54" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="202" spans="1:1" ht="15">
-      <c r="A202" s="56" t="s">
+    <row r="210" spans="1:1" ht="15">
+      <c r="A210" s="54"/>
+    </row>
+    <row r="211" spans="1:1" ht="16.5">
+      <c r="A211" s="55" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="203" spans="1:1" ht="15">
-      <c r="A203" s="56" t="s">
+    <row r="212" spans="1:1" ht="15">
+      <c r="A212" s="54" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="15">
-      <c r="A204" s="56" t="s">
+    <row r="213" spans="1:1" ht="15">
+      <c r="A213" s="54" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="205" spans="1:1" ht="15">
-      <c r="A205" s="56" t="s">
+    <row r="214" spans="1:1" ht="15">
+      <c r="A214" s="54" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="206" spans="1:1" ht="15">
-      <c r="A206" s="56" t="s">
+    <row r="215" spans="1:1" ht="15">
+      <c r="A215" s="54" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="207" spans="1:1" ht="15">
-      <c r="A207" s="56" t="s">
+    <row r="216" spans="1:1" ht="15">
+      <c r="A216" s="54"/>
+    </row>
+    <row r="217" spans="1:1" ht="16.5">
+      <c r="A217" s="55" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="208" spans="1:1" ht="15">
-      <c r="A208" s="56" t="s">
+    <row r="218" spans="1:1" ht="15">
+      <c r="A218" s="54" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="15">
-      <c r="A209" s="56" t="s">
+    <row r="219" spans="1:1" ht="15">
+      <c r="A219" s="54" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="15">
-      <c r="A210" s="56"/>
-    </row>
-    <row r="211" spans="1:1" ht="16.5">
-      <c r="A211" s="57" t="s">
+    <row r="220" spans="1:1" ht="15">
+      <c r="A220" s="54"/>
+    </row>
+    <row r="221" spans="1:1" ht="16.5">
+      <c r="A221" s="55" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="15">
-      <c r="A212" s="56" t="s">
+    <row r="222" spans="1:1" ht="15">
+      <c r="A222" s="54" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="213" spans="1:1" ht="15">
-      <c r="A213" s="56" t="s">
+    <row r="223" spans="1:1" ht="15">
+      <c r="A223" s="54" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="214" spans="1:1" ht="15">
-      <c r="A214" s="56" t="s">
+    <row r="224" spans="1:1" ht="15">
+      <c r="A224" s="54" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="15">
-      <c r="A215" s="56" t="s">
+    <row r="225" spans="1:1" ht="15">
+      <c r="A225" s="54" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="15">
-      <c r="A216" s="56"/>
-    </row>
-    <row r="217" spans="1:1" ht="16.5">
-      <c r="A217" s="57" t="s">
+    <row r="226" spans="1:1" ht="15">
+      <c r="A226" s="54" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="218" spans="1:1" ht="15">
-      <c r="A218" s="56" t="s">
+    <row r="227" spans="1:1" ht="15">
+      <c r="A227" s="54" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="219" spans="1:1" ht="15">
-      <c r="A219" s="56" t="s">
+    <row r="228" spans="1:1" ht="15">
+      <c r="A228" s="54" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="220" spans="1:1" ht="15">
-      <c r="A220" s="56"/>
-    </row>
-    <row r="221" spans="1:1" ht="16.5">
-      <c r="A221" s="57" t="s">
+    <row r="229" spans="1:1" ht="15">
+      <c r="A229" s="54" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="222" spans="1:1" ht="15">
-      <c r="A222" s="56" t="s">
+    <row r="230" spans="1:1" ht="15">
+      <c r="A230" s="54" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="223" spans="1:1" ht="15">
-      <c r="A223" s="56" t="s">
+    <row r="231" spans="1:1" ht="15">
+      <c r="A231" s="54"/>
+    </row>
+    <row r="232" spans="1:1" ht="16.5">
+      <c r="A232" s="55" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="224" spans="1:1" ht="15">
-      <c r="A224" s="56" t="s">
+    <row r="233" spans="1:1" ht="15">
+      <c r="A233" s="54" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="225" spans="1:1" ht="15">
-      <c r="A225" s="56" t="s">
+    <row r="234" spans="1:1" ht="15">
+      <c r="A234" s="54"/>
+    </row>
+    <row r="235" spans="1:1" ht="16.5">
+      <c r="A235" s="55" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="15">
-      <c r="A226" s="56" t="s">
+    <row r="236" spans="1:1" ht="15">
+      <c r="A236" s="54" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="227" spans="1:1" ht="15">
-      <c r="A227" s="56" t="s">
+    <row r="237" spans="1:1" ht="15">
+      <c r="A237" s="54" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="15">
-      <c r="A228" s="56" t="s">
+    <row r="239" spans="1:1" ht="16.5">
+      <c r="A239" s="55" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="229" spans="1:1" ht="15">
-      <c r="A229" s="56" t="s">
+    <row r="240" spans="1:1">
+      <c r="A240" s="56" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="230" spans="1:1" ht="15">
-      <c r="A230" s="56" t="s">
+    <row r="241" spans="1:1">
+      <c r="A241" s="56" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="15">
-      <c r="A231" s="56"/>
-    </row>
-    <row r="232" spans="1:1" ht="16.5">
-      <c r="A232" s="57" t="s">
+    <row r="242" spans="1:1">
+      <c r="A242" s="56" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="233" spans="1:1" ht="15">
-      <c r="A233" s="56" t="s">
+    <row r="243" spans="1:1">
+      <c r="A243" s="56" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="234" spans="1:1" ht="15">
-      <c r="A234" s="56"/>
-    </row>
-    <row r="235" spans="1:1" ht="16.5">
-      <c r="A235" s="57" t="s">
+    <row r="244" spans="1:1">
+      <c r="A244" s="56" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="236" spans="1:1" ht="15">
-      <c r="A236" s="56" t="s">
+    <row r="245" spans="1:1">
+      <c r="A245" s="56" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="237" spans="1:1" ht="15">
-      <c r="A237" s="56" t="s">
+    <row r="247" spans="1:1" ht="16.5">
+      <c r="A247" s="55" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="239" spans="1:1" ht="16.5">
-      <c r="A239" s="57" t="s">
+    <row r="249" spans="1:1" ht="16.5">
+      <c r="A249" s="55" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="240" spans="1:1">
-      <c r="A240" s="58" t="s">
+    <row r="251" spans="1:1" ht="16.5">
+      <c r="A251" s="55" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="241" spans="1:1">
-      <c r="A241" s="58" t="s">
+    <row r="252" spans="1:1">
+      <c r="A252" s="59" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="242" spans="1:1">
-      <c r="A242" s="58" t="s">
+    <row r="253" spans="1:1">
+      <c r="A253" s="59" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="243" spans="1:1">
-      <c r="A243" s="58" t="s">
+    <row r="254" spans="1:1">
+      <c r="A254" s="59" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="244" spans="1:1">
-      <c r="A244" s="58" t="s">
+    <row r="255" spans="1:1">
+      <c r="A255" s="59" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="245" spans="1:1">
-      <c r="A245" s="58" t="s">
+    <row r="256" spans="1:1">
+      <c r="A256" s="59" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="247" spans="1:1" ht="16.5">
-      <c r="A247" s="57" t="s">
+    <row r="257" spans="1:1">
+      <c r="A257" s="60" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="249" spans="1:1" ht="16.5">
-      <c r="A249" s="57" t="s">
+    <row r="258" spans="1:1">
+      <c r="A258" s="59" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="251" spans="1:1" ht="16.5">
-      <c r="A251" s="57" t="s">
+    <row r="259" spans="1:1">
+      <c r="A259" s="59" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="252" spans="1:1">
-      <c r="A252" s="61" t="s">
+    <row r="260" spans="1:1">
+      <c r="A260" s="59" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1">
-      <c r="A253" s="61" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1">
-      <c r="A254" s="61" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1">
-      <c r="A255" s="61" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1">
-      <c r="A256" s="61" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1">
-      <c r="A257" s="62" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1">
-      <c r="A258" s="61" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1">
-      <c r="A259" s="61" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1">
-      <c r="A260" s="61" t="s">
-        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>